<commit_message>
Update doc and excel, update 03.
</commit_message>
<xml_diff>
--- a/dbFinal.xlsx
+++ b/dbFinal.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\3 科研\3 横向课题\2 杭电\4 娱乐指数\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WorkSpace\movie-crawer\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7965"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7970"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="203">
   <si>
     <t xml:space="preserve">ActorID     </t>
   </si>
@@ -97,10 +97,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>(来源:CBO)(http://www.cbooo.cn/c/6)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>CompanyID</t>
   </si>
   <si>
@@ -147,24 +143,9 @@
     <t>MovieLength</t>
   </si>
   <si>
-    <t xml:space="preserve">MovieReleasetime   </t>
-  </si>
-  <si>
     <t xml:space="preserve">MovieStandard      </t>
   </si>
   <si>
-    <t xml:space="preserve">MovieSumboxoffice  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MovieAvgprice      </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MovieAvgpeople     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MovieWomindex      </t>
-  </si>
-  <si>
     <t>Float</t>
   </si>
   <si>
@@ -244,9 +225,6 @@
     <t>BoxOfficeDate</t>
   </si>
   <si>
-    <t xml:space="preserve">Boxoffice     </t>
-  </si>
-  <si>
     <t xml:space="preserve">BoxOfficeAvgpeople       </t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -489,13 +467,7 @@
     <t>放映场次</t>
   </si>
   <si>
-    <t>CinemaSumboxoffice</t>
-  </si>
-  <si>
     <t>总票房数</t>
-  </si>
-  <si>
-    <t>CinemaSumpeople</t>
   </si>
   <si>
     <t>总观影人数</t>
@@ -787,16 +759,52 @@
     </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BoxOffice     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MovieAvgPrice      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MovieAvgPeople     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MovieWomIndex      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MovieSumBoxOffice  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MovieReleaseTime   </t>
+  </si>
+  <si>
+    <t>CinemaParking</t>
+  </si>
+  <si>
+    <t>影院是否有停车位</t>
+  </si>
+  <si>
+    <t>bit</t>
+  </si>
+  <si>
+    <t>CinemaSumBoxOffice</t>
+  </si>
+  <si>
+    <t>CinemaSumPeople</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -816,7 +824,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -824,7 +832,7 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -832,7 +840,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -840,7 +848,7 @@
     <font>
       <sz val="10.5"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -959,23 +967,23 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1298,24 +1306,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G152" sqref="G152"/>
+    <sheetView tabSelected="1" topLeftCell="A98" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A116" sqref="A116"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="24.625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="23.5" style="7" customWidth="1"/>
+    <col min="1" max="1" width="24.6328125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="23.453125" style="7" customWidth="1"/>
     <col min="3" max="4" width="9" style="7"/>
     <col min="5" max="5" width="28" style="7" customWidth="1"/>
-    <col min="7" max="7" width="14.25" customWidth="1"/>
-    <col min="8" max="8" width="18.625" customWidth="1"/>
-    <col min="9" max="9" width="22.375" customWidth="1"/>
-    <col min="10" max="10" width="19.5" customWidth="1"/>
-    <col min="11" max="11" width="17.125" customWidth="1"/>
+    <col min="7" max="7" width="14.26953125" customWidth="1"/>
+    <col min="8" max="8" width="18.6328125" customWidth="1"/>
+    <col min="9" max="9" width="22.36328125" customWidth="1"/>
+    <col min="10" max="10" width="19.453125" customWidth="1"/>
+    <col min="11" max="11" width="17.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="18.5">
       <c r="A1" s="19" t="s">
         <v>14</v>
       </c>
@@ -1324,7 +1332,7 @@
       <c r="D1" s="19"/>
       <c r="E1" s="19"/>
     </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" s="1" customFormat="1" ht="18.5">
       <c r="A2" s="19" t="s">
         <v>15</v>
       </c>
@@ -1333,7 +1341,7 @@
       <c r="D2" s="19"/>
       <c r="E2" s="19"/>
     </row>
-    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="18.5">
       <c r="A3" s="13" t="s">
         <v>9</v>
       </c>
@@ -1350,7 +1358,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
@@ -1367,7 +1375,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" s="7" t="s">
         <v>4</v>
       </c>
@@ -1378,7 +1386,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
@@ -1389,7 +1397,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" s="7" t="s">
         <v>8</v>
       </c>
@@ -1400,17 +1408,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="18.5">
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="B9" s="8"/>
     </row>
-    <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="18.5">
       <c r="A10" s="19" t="s">
         <v>19</v>
       </c>
@@ -1419,16 +1427,16 @@
       <c r="D10" s="19"/>
       <c r="E10" s="19"/>
     </row>
-    <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="18.5">
       <c r="A11" s="19" t="s">
-        <v>20</v>
+        <v>191</v>
       </c>
       <c r="B11" s="19"/>
       <c r="C11" s="19"/>
       <c r="D11" s="19"/>
       <c r="E11" s="19"/>
     </row>
-    <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="18.5">
       <c r="A12" s="13" t="s">
         <v>9</v>
       </c>
@@ -1445,12 +1453,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>21</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>22</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>1</v>
@@ -1462,12 +1470,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="18.5">
       <c r="A14" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>23</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>24</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>5</v>
@@ -1475,25 +1483,25 @@
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="18.5">
       <c r="A15" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>26</v>
-      </c>
       <c r="C15" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="18.5">
       <c r="A16" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>27</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>28</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>5</v>
@@ -1501,41 +1509,41 @@
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="15"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-    </row>
-    <row r="20" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9">
+      <c r="A17" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="14"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+    </row>
+    <row r="20" spans="1:9" ht="18.5">
       <c r="A20" s="19" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B20" s="19"/>
       <c r="C20" s="19"/>
       <c r="D20" s="19"/>
       <c r="E20" s="19"/>
     </row>
-    <row r="21" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="18.5">
       <c r="A21" s="19" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B21" s="19"/>
       <c r="C21" s="19"/>
       <c r="D21" s="19"/>
       <c r="E21" s="19"/>
     </row>
-    <row r="22" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" ht="18.5">
       <c r="A22" s="13" t="s">
         <v>9</v>
       </c>
@@ -1553,12 +1561,12 @@
       </c>
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9">
       <c r="A23" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>1</v>
@@ -1571,138 +1579,138 @@
       </c>
       <c r="I23" s="3"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9">
       <c r="A24" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>5</v>
       </c>
       <c r="I24" s="3"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9">
       <c r="A25" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>5</v>
       </c>
       <c r="I25" s="3"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9">
       <c r="A26" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>5</v>
       </c>
       <c r="I26" s="3"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9">
       <c r="A27" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I27" s="3"/>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I28" s="3"/>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="I27" s="3"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="I28" s="3"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="7" t="s">
-        <v>37</v>
-      </c>
       <c r="B29" s="8" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>5</v>
       </c>
       <c r="I29" s="3"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9">
       <c r="A30" s="7" t="s">
-        <v>38</v>
+        <v>196</v>
       </c>
       <c r="B30" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I30" s="3"/>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I31" s="3"/>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I32" s="3"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="B34" s="8"/>
+    </row>
+    <row r="36" spans="1:5" ht="18.5">
+      <c r="A36" s="19" t="s">
         <v>50</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="I30" s="3"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="I31" s="3"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="I32" s="3"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B34" s="8"/>
-    </row>
-    <row r="36" spans="1:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="A36" s="19" t="s">
-        <v>56</v>
       </c>
       <c r="B36" s="19"/>
       <c r="C36" s="19"/>
       <c r="D36" s="19"/>
       <c r="E36" s="19"/>
     </row>
-    <row r="37" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" ht="18.5">
       <c r="A37" s="19" t="s">
         <v>15</v>
       </c>
@@ -1711,7 +1719,7 @@
       <c r="D37" s="19"/>
       <c r="E37" s="19"/>
     </row>
-    <row r="38" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" ht="18.5">
       <c r="A38" s="13" t="s">
         <v>9</v>
       </c>
@@ -1728,12 +1736,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5">
       <c r="A39" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>1</v>
@@ -1745,12 +1753,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5">
       <c r="A40" s="7" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C40" s="7" t="s">
         <v>1</v>
@@ -1762,47 +1770,47 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5">
       <c r="A41" s="7" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C41" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5">
       <c r="A42" s="7" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C42" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" ht="18.5">
       <c r="A45" s="19" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B45" s="19"/>
       <c r="C45" s="19"/>
       <c r="D45" s="19"/>
       <c r="E45" s="19"/>
     </row>
-    <row r="46" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" ht="18.5">
       <c r="A46" s="19" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B46" s="19"/>
       <c r="C46" s="19"/>
       <c r="D46" s="19"/>
       <c r="E46" s="19"/>
     </row>
-    <row r="47" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" ht="18.5">
       <c r="A47" s="13" t="s">
         <v>9</v>
       </c>
@@ -1819,12 +1827,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5">
       <c r="A48" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C48" s="7" t="s">
         <v>1</v>
@@ -1836,12 +1844,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5">
       <c r="A49" s="7" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C49" s="7" t="s">
         <v>1</v>
@@ -1853,47 +1861,47 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5">
       <c r="A50" s="7" t="s">
-        <v>66</v>
+        <v>192</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C50" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5">
       <c r="A51" s="7" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C51" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" ht="18.5">
       <c r="A54" s="19" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B54" s="19"/>
       <c r="C54" s="19"/>
       <c r="D54" s="19"/>
       <c r="E54" s="19"/>
     </row>
-    <row r="55" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" ht="18.5">
       <c r="A55" s="19" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B55" s="19"/>
       <c r="C55" s="19"/>
       <c r="D55" s="19"/>
       <c r="E55" s="19"/>
     </row>
-    <row r="56" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" ht="18.5">
       <c r="A56" s="13" t="s">
         <v>9</v>
       </c>
@@ -1910,81 +1918,81 @@
         <v>13</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="B57" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="C57" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="D57" s="16" t="s">
+    <row r="57" spans="1:5">
+      <c r="A57" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B57" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C57" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D57" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E57" s="16" t="s">
+      <c r="E57" s="15" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="B58" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C58" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="D58" s="16" t="s">
+    <row r="58" spans="1:5">
+      <c r="A58" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B58" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C58" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D58" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E58" s="16" t="s">
+      <c r="E58" s="15" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="B59" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="C59" s="16" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="B60" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="C60" s="16" t="s">
+    <row r="59" spans="1:5">
+      <c r="A59" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B59" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C59" s="15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B60" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C60" s="15" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" ht="18.5">
       <c r="A63" s="19" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B63" s="19"/>
       <c r="C63" s="19"/>
       <c r="D63" s="19"/>
       <c r="E63" s="19"/>
     </row>
-    <row r="64" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" ht="18.5">
       <c r="A64" s="19" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B64" s="19"/>
       <c r="C64" s="19"/>
       <c r="D64" s="19"/>
       <c r="E64" s="19"/>
     </row>
-    <row r="65" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" ht="18.5">
       <c r="A65" s="13" t="s">
         <v>9</v>
       </c>
@@ -2001,12 +2009,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5">
       <c r="A66" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C66" s="7" t="s">
         <v>1</v>
@@ -2018,12 +2026,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5">
       <c r="A67" s="7" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C67" s="7" t="s">
         <v>1</v>
@@ -2035,12 +2043,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5">
       <c r="A68" s="7" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C68" s="7" t="s">
         <v>1</v>
@@ -2052,36 +2060,36 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5">
       <c r="A69" s="7" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C69" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="A72" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="B72" s="18"/>
-      <c r="C72" s="18"/>
-      <c r="D72" s="18"/>
-      <c r="E72" s="18"/>
-    </row>
-    <row r="73" spans="1:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="A73" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="B73" s="18"/>
-      <c r="C73" s="18"/>
-      <c r="D73" s="18"/>
-      <c r="E73" s="18"/>
-    </row>
-    <row r="74" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" ht="18.5">
+      <c r="A72" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="B72" s="17"/>
+      <c r="C72" s="17"/>
+      <c r="D72" s="17"/>
+      <c r="E72" s="17"/>
+    </row>
+    <row r="73" spans="1:5" ht="18.5">
+      <c r="A73" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B73" s="17"/>
+      <c r="C73" s="17"/>
+      <c r="D73" s="17"/>
+      <c r="E73" s="17"/>
+    </row>
+    <row r="74" spans="1:5" ht="18.5">
       <c r="A74" s="13" t="s">
         <v>9</v>
       </c>
@@ -2098,12 +2106,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5">
       <c r="A75" s="7" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C75" s="7" t="s">
         <v>1</v>
@@ -2115,12 +2123,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5">
       <c r="A76" s="7" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C76" s="7" t="s">
         <v>1</v>
@@ -2129,105 +2137,116 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5">
       <c r="A77" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B80" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="B77" s="7" t="s">
+      <c r="C80" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11">
+      <c r="A81" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="C77" s="7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A78" s="7" t="s">
+      <c r="B81" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B78" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="C78" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A79" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="B79" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="C79" s="7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A80" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="B80" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="C80" s="7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A81" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="B81" s="7" t="s">
-        <v>100</v>
-      </c>
       <c r="C81" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E81" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11">
       <c r="A82" s="7" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="C82" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11">
       <c r="A83" s="7" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C83" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="1:11" ht="18" x14ac:dyDescent="0.2">
-      <c r="A86" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="B86" s="18"/>
-      <c r="C86" s="18"/>
-      <c r="D86" s="18"/>
-      <c r="E86" s="18"/>
-    </row>
-    <row r="87" spans="1:11" ht="18" x14ac:dyDescent="0.2">
-      <c r="A87" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="B87" s="18"/>
-      <c r="C87" s="18"/>
-      <c r="D87" s="18"/>
-      <c r="E87" s="18"/>
-    </row>
-    <row r="88" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11">
+      <c r="A84" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="C84" s="7" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" ht="18.5">
+      <c r="A86" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="B86" s="17"/>
+      <c r="C86" s="17"/>
+      <c r="D86" s="17"/>
+      <c r="E86" s="17"/>
+    </row>
+    <row r="87" spans="1:11" ht="18.5">
+      <c r="A87" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="B87" s="17"/>
+      <c r="C87" s="17"/>
+      <c r="D87" s="17"/>
+      <c r="E87" s="17"/>
+    </row>
+    <row r="88" spans="1:11" ht="18.5">
       <c r="A88" s="13" t="s">
         <v>9</v>
       </c>
@@ -2244,31 +2263,31 @@
         <v>13</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A89" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="B89" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="C89" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="D89" s="16" t="s">
+    <row r="89" spans="1:11">
+      <c r="A89" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="B89" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="C89" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D89" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E89" s="16" t="s">
+      <c r="E89" s="15" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A90" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="B90" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="C90" s="16" t="s">
+    <row r="90" spans="1:11">
+      <c r="A90" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="B90" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C90" s="15" t="s">
         <v>1</v>
       </c>
       <c r="G90" s="9"/>
@@ -2277,78 +2296,78 @@
       <c r="J90" s="10"/>
       <c r="K90" s="10"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A91" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="B91" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="C91" s="16" t="s">
-        <v>29</v>
+    <row r="91" spans="1:11">
+      <c r="A91" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="B91" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="C91" s="15" t="s">
+        <v>28</v>
       </c>
       <c r="G91" s="9"/>
       <c r="H91" s="10"/>
       <c r="I91" s="9"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A92" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="B92" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="C92" s="16" t="s">
+    <row r="92" spans="1:11">
+      <c r="A92" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="B92" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="C92" s="15" t="s">
         <v>5</v>
       </c>
       <c r="G92" s="9"/>
       <c r="H92" s="10"/>
       <c r="I92" s="9"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A93" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="B93" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="C93" s="16" t="s">
+    <row r="93" spans="1:11">
+      <c r="A93" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="B93" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C93" s="15" t="s">
         <v>5</v>
       </c>
       <c r="G93" s="9"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A94" s="16"/>
-      <c r="B94" s="16"/>
-      <c r="C94" s="16"/>
+    <row r="94" spans="1:11">
+      <c r="A94" s="15"/>
+      <c r="B94" s="15"/>
+      <c r="C94" s="15"/>
       <c r="G94" s="9"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A95" s="16"/>
-      <c r="B95" s="16"/>
-      <c r="C95" s="16"/>
+    <row r="95" spans="1:11">
+      <c r="A95" s="15"/>
+      <c r="B95" s="15"/>
+      <c r="C95" s="15"/>
       <c r="G95" s="9"/>
     </row>
-    <row r="96" spans="1:11" ht="18" x14ac:dyDescent="0.2">
-      <c r="A96" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="B96" s="18"/>
-      <c r="C96" s="18"/>
-      <c r="D96" s="18"/>
-      <c r="E96" s="18"/>
+    <row r="96" spans="1:11" ht="18.5">
+      <c r="A96" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="B96" s="17"/>
+      <c r="C96" s="17"/>
+      <c r="D96" s="17"/>
+      <c r="E96" s="17"/>
       <c r="G96" s="9"/>
     </row>
-    <row r="97" spans="1:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="A97" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="B97" s="18"/>
-      <c r="C97" s="18"/>
-      <c r="D97" s="18"/>
-      <c r="E97" s="18"/>
-    </row>
-    <row r="98" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:5" ht="18.5">
+      <c r="A97" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="B97" s="17"/>
+      <c r="C97" s="17"/>
+      <c r="D97" s="17"/>
+      <c r="E97" s="17"/>
+    </row>
+    <row r="98" spans="1:5" ht="18.5">
       <c r="A98" s="13" t="s">
         <v>9</v>
       </c>
@@ -2365,15 +2384,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A99" s="16" t="s">
-        <v>115</v>
+    <row r="99" spans="1:5">
+      <c r="A99" s="15" t="s">
+        <v>108</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="D99" s="7" t="s">
         <v>2</v>
@@ -2382,96 +2401,96 @@
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A100" s="16" t="s">
+    <row r="100" spans="1:5">
+      <c r="A100" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="B100" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="C100" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B101" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C101" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
+      <c r="A102" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B102" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C102" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
+      <c r="A103" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B103" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="B100" s="16" t="s">
+      <c r="C103" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="C100" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A101" s="7" t="s">
+    </row>
+    <row r="104" spans="1:5">
+      <c r="A104" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="B101" s="7" t="s">
+      <c r="B104" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="C101" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A102" s="7" t="s">
+      <c r="C104" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="B102" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C102" s="7" t="s">
+    </row>
+    <row r="105" spans="1:5">
+      <c r="A105" s="7" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A103" s="7" t="s">
+      <c r="B105" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="B103" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="C103" s="7" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A104" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="B104" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="C104" s="7" t="s">
+      <c r="C105" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
+      <c r="A106" s="15"/>
+      <c r="B106" s="15"/>
+      <c r="C106" s="15"/>
+    </row>
+    <row r="108" spans="1:5" ht="18.5">
+      <c r="A108" s="17" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A105" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="B105" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="C105" s="7" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A106" s="16"/>
-      <c r="B106" s="16"/>
-      <c r="C106" s="16"/>
-    </row>
-    <row r="108" spans="1:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="A108" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="B108" s="18"/>
-      <c r="C108" s="18"/>
-      <c r="D108" s="18"/>
-      <c r="E108" s="18"/>
-    </row>
-    <row r="109" spans="1:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="A109" s="18" t="s">
-        <v>168</v>
-      </c>
-      <c r="B109" s="18"/>
-      <c r="C109" s="18"/>
-      <c r="D109" s="18"/>
-      <c r="E109" s="18"/>
-    </row>
-    <row r="110" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="B108" s="17"/>
+      <c r="C108" s="17"/>
+      <c r="D108" s="17"/>
+      <c r="E108" s="17"/>
+    </row>
+    <row r="109" spans="1:5" ht="18.5">
+      <c r="A109" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="B109" s="17"/>
+      <c r="C109" s="17"/>
+      <c r="D109" s="17"/>
+      <c r="E109" s="17"/>
+    </row>
+    <row r="110" spans="1:5" ht="18.5">
       <c r="A110" s="13" t="s">
         <v>9</v>
       </c>
@@ -2488,12 +2507,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:5">
       <c r="A111" s="7" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C111" s="7" t="s">
         <v>1</v>
@@ -2505,12 +2524,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:5">
       <c r="A112" s="7" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="C112" s="7" t="s">
         <v>1</v>
@@ -2522,12 +2541,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:5">
       <c r="A113" s="7" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C113" s="7" t="s">
         <v>1</v>
@@ -2539,58 +2558,58 @@
         <v>3</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:5">
       <c r="A114" s="7" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="B114" s="7" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="C114" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:5">
       <c r="A115" s="7" t="s">
-        <v>141</v>
+        <v>201</v>
       </c>
       <c r="B115" s="7" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="C115" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:5">
       <c r="A116" s="7" t="s">
-        <v>143</v>
+        <v>202</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="C116" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="A119" s="18" t="s">
-        <v>146</v>
-      </c>
-      <c r="B119" s="18"/>
-      <c r="C119" s="18"/>
-      <c r="D119" s="18"/>
-      <c r="E119" s="18"/>
-    </row>
-    <row r="120" spans="1:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="A120" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="B120" s="18"/>
-      <c r="C120" s="18"/>
-      <c r="D120" s="18"/>
-      <c r="E120" s="18"/>
-    </row>
-    <row r="121" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:5" ht="18.5">
+      <c r="A119" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="B119" s="17"/>
+      <c r="C119" s="17"/>
+      <c r="D119" s="17"/>
+      <c r="E119" s="17"/>
+    </row>
+    <row r="120" spans="1:5" ht="18.5">
+      <c r="A120" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="B120" s="17"/>
+      <c r="C120" s="17"/>
+      <c r="D120" s="17"/>
+      <c r="E120" s="17"/>
+    </row>
+    <row r="121" spans="1:5" ht="18.5">
       <c r="A121" s="13" t="s">
         <v>9</v>
       </c>
@@ -2607,12 +2626,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:5">
       <c r="A122" s="7" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B122" s="7" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C122" s="7" t="s">
         <v>1</v>
@@ -2624,12 +2643,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:5">
       <c r="A123" s="7" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B123" s="7" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C123" s="7" t="s">
         <v>1</v>
@@ -2641,12 +2660,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:5">
       <c r="A124" s="7" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="B124" s="7" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="C124" s="7" t="s">
         <v>1</v>
@@ -2658,12 +2677,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:5">
       <c r="A125" s="7" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B125" s="7" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="C125" s="7" t="s">
         <v>1</v>
@@ -2675,12 +2694,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:5">
       <c r="A126" s="7" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="B126" s="7" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C126" s="7" t="s">
         <v>1</v>
@@ -2692,102 +2711,102 @@
         <v>3</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:5">
       <c r="A127" s="7" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B127" s="7" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="C127" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:5">
       <c r="A128" s="7" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="B128" s="7" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="C128" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:15">
       <c r="A129" s="7" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="B129" s="7" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="C129" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:15">
       <c r="A130" s="7" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="B130" s="7" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="C130" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:15">
       <c r="A131" s="7" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="B131" s="7" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="C131" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="132" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:15">
       <c r="A132" s="7" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="B132" s="7" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="C132" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:15">
       <c r="A133" s="7" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="B133" s="7" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="C133" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="136" spans="1:15" ht="18" x14ac:dyDescent="0.2">
-      <c r="A136" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="B136" s="17"/>
-      <c r="C136" s="17"/>
-      <c r="D136" s="17"/>
-      <c r="E136" s="17"/>
-    </row>
-    <row r="137" spans="1:15" ht="18" x14ac:dyDescent="0.2">
-      <c r="A137" s="17" t="s">
-        <v>181</v>
-      </c>
-      <c r="B137" s="17"/>
-      <c r="C137" s="17"/>
-      <c r="D137" s="17"/>
-      <c r="E137" s="17"/>
-    </row>
-    <row r="138" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:15" ht="18.5">
+      <c r="A136" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="B136" s="18"/>
+      <c r="C136" s="18"/>
+      <c r="D136" s="18"/>
+      <c r="E136" s="18"/>
+    </row>
+    <row r="137" spans="1:15" ht="18.5">
+      <c r="A137" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="B137" s="18"/>
+      <c r="C137" s="18"/>
+      <c r="D137" s="18"/>
+      <c r="E137" s="18"/>
+    </row>
+    <row r="138" spans="1:15" ht="18.5">
       <c r="A138" s="13" t="s">
         <v>9</v>
       </c>
@@ -2804,20 +2823,20 @@
         <v>13</v>
       </c>
     </row>
-    <row r="139" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A139" s="16" t="s">
-        <v>169</v>
-      </c>
-      <c r="B139" s="16" t="s">
-        <v>183</v>
+    <row r="139" spans="1:15">
+      <c r="A139" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="B139" s="15" t="s">
+        <v>174</v>
       </c>
       <c r="C139" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="D139" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="D139" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E139" s="16" t="s">
+      <c r="E139" s="15" t="s">
         <v>3</v>
       </c>
       <c r="H139" s="9"/>
@@ -2825,37 +2844,37 @@
       <c r="K139" s="10"/>
       <c r="L139" s="10"/>
     </row>
-    <row r="140" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A140" s="16" t="s">
-        <v>179</v>
+    <row r="140" spans="1:15">
+      <c r="A140" s="15" t="s">
+        <v>170</v>
       </c>
       <c r="B140" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="C140" s="16" t="s">
-        <v>170</v>
-      </c>
-      <c r="E140" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C140" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="E140" s="15" t="s">
         <v>3</v>
       </c>
       <c r="H140" s="9"/>
       <c r="J140" s="9"/>
       <c r="L140" s="10"/>
     </row>
-    <row r="141" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A141" s="16" t="s">
-        <v>171</v>
-      </c>
-      <c r="B141" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="C141" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="D141" s="16" t="s">
+    <row r="141" spans="1:15">
+      <c r="A141" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B141" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="C141" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="D141" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E141" s="16" t="s">
+      <c r="E141" s="15" t="s">
         <v>3</v>
       </c>
       <c r="H141" s="9"/>
@@ -2864,20 +2883,20 @@
       <c r="K141" s="10"/>
       <c r="L141" s="10"/>
     </row>
-    <row r="142" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A142" s="16" t="s">
-        <v>174</v>
-      </c>
-      <c r="B142" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="C142" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="D142" s="16" t="s">
+    <row r="142" spans="1:15">
+      <c r="A142" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="B142" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="C142" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="D142" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E142" s="16" t="s">
+      <c r="E142" s="15" t="s">
         <v>3</v>
       </c>
       <c r="H142" s="9"/>
@@ -2886,49 +2905,49 @@
       <c r="K142" s="10"/>
       <c r="L142" s="10"/>
     </row>
-    <row r="143" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A143" s="16" t="s">
-        <v>176</v>
-      </c>
-      <c r="B143" s="16" t="s">
-        <v>177</v>
-      </c>
-      <c r="C143" s="16" t="s">
-        <v>170</v>
+    <row r="143" spans="1:15">
+      <c r="A143" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="B143" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="C143" s="15" t="s">
+        <v>161</v>
       </c>
       <c r="H143" s="9"/>
       <c r="I143" s="10"/>
       <c r="J143" s="9"/>
       <c r="O143" s="10"/>
     </row>
-    <row r="144" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A144" s="16"/>
-      <c r="B144" s="16"/>
-      <c r="C144" s="16"/>
+    <row r="144" spans="1:15">
+      <c r="A144" s="15"/>
+      <c r="B144" s="15"/>
+      <c r="C144" s="15"/>
       <c r="H144" s="9"/>
       <c r="I144" s="10"/>
       <c r="J144" s="9"/>
       <c r="O144" s="10"/>
     </row>
-    <row r="146" spans="1:11" ht="18" x14ac:dyDescent="0.2">
-      <c r="A146" s="20" t="s">
-        <v>184</v>
-      </c>
-      <c r="B146" s="20"/>
-      <c r="C146" s="20"/>
-      <c r="D146" s="20"/>
-      <c r="E146" s="20"/>
-    </row>
-    <row r="147" spans="1:11" ht="18" x14ac:dyDescent="0.2">
-      <c r="A147" s="20" t="s">
-        <v>185</v>
-      </c>
-      <c r="B147" s="20"/>
-      <c r="C147" s="20"/>
-      <c r="D147" s="20"/>
-      <c r="E147" s="20"/>
-    </row>
-    <row r="148" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:11" ht="18.5">
+      <c r="A146" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="B146" s="16"/>
+      <c r="C146" s="16"/>
+      <c r="D146" s="16"/>
+      <c r="E146" s="16"/>
+    </row>
+    <row r="147" spans="1:11" ht="18.5">
+      <c r="A147" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="B147" s="16"/>
+      <c r="C147" s="16"/>
+      <c r="D147" s="16"/>
+      <c r="E147" s="16"/>
+    </row>
+    <row r="148" spans="1:11" ht="18.5">
       <c r="A148" s="13" t="s">
         <v>9</v>
       </c>
@@ -2945,15 +2964,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:11">
       <c r="A149" s="11" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="B149" s="12" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="C149" s="11" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="D149" s="12" t="s">
         <v>2</v>
@@ -2962,28 +2981,28 @@
         <v>3</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:11">
       <c r="A150" s="11" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="B150" s="11" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="C150" s="11" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="D150" s="2"/>
       <c r="E150" s="2"/>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:11">
       <c r="A151" s="11" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B151" s="12" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="C151" s="11" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="D151" s="2"/>
       <c r="E151" s="2"/>
@@ -2993,15 +3012,15 @@
       <c r="J151" s="10"/>
       <c r="K151" s="10"/>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:11">
       <c r="A152" s="11" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="B152" s="11" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="C152" s="11" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="D152" s="2"/>
       <c r="E152" s="2"/>
@@ -3009,15 +3028,15 @@
       <c r="H152" s="9"/>
       <c r="I152" s="9"/>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:11">
       <c r="A153" s="11" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="B153" s="11" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="C153" s="11" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="D153" s="2"/>
       <c r="E153" s="2"/>
@@ -3025,15 +3044,15 @@
       <c r="H153" s="10"/>
       <c r="I153" s="9"/>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:11">
       <c r="A154" s="11" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="B154" s="11" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="C154" s="11" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="D154" s="2"/>
       <c r="E154" s="2"/>
@@ -3041,15 +3060,15 @@
       <c r="H154" s="9"/>
       <c r="I154" s="9"/>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:11">
       <c r="A155" s="11" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="C155" s="11" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="D155" s="2"/>
       <c r="E155" s="2"/>
@@ -3057,15 +3076,15 @@
       <c r="H155" s="9"/>
       <c r="I155" s="9"/>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:11">
       <c r="A156" s="11" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B156" s="12" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="D156" s="2"/>
       <c r="E156" s="2"/>
@@ -3073,37 +3092,38 @@
       <c r="H156" s="9"/>
       <c r="I156" s="9"/>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:11">
       <c r="A157" s="11" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="B157" s="11" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="D157" s="2"/>
       <c r="E157" s="2"/>
       <c r="G157" s="9"/>
       <c r="I157" s="9"/>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:11">
       <c r="G158" s="9"/>
       <c r="H158" s="10"/>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:11">
       <c r="G159" s="9"/>
       <c r="H159" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="A147:E147"/>
-    <mergeCell ref="A119:E119"/>
-    <mergeCell ref="A120:E120"/>
-    <mergeCell ref="A136:E136"/>
-    <mergeCell ref="A137:E137"/>
-    <mergeCell ref="A146:E146"/>
+    <mergeCell ref="A46:E46"/>
+    <mergeCell ref="A54:E54"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A17:E17"/>
     <mergeCell ref="A20:E20"/>
     <mergeCell ref="A63:E63"/>
     <mergeCell ref="A64:E64"/>
@@ -3115,18 +3135,17 @@
     <mergeCell ref="A87:E87"/>
     <mergeCell ref="A96:E96"/>
     <mergeCell ref="A97:E97"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A17:E17"/>
     <mergeCell ref="A55:E55"/>
     <mergeCell ref="A21:E21"/>
     <mergeCell ref="A36:E36"/>
     <mergeCell ref="A37:E37"/>
     <mergeCell ref="A45:E45"/>
-    <mergeCell ref="A46:E46"/>
-    <mergeCell ref="A54:E54"/>
+    <mergeCell ref="A147:E147"/>
+    <mergeCell ref="A119:E119"/>
+    <mergeCell ref="A120:E120"/>
+    <mergeCell ref="A136:E136"/>
+    <mergeCell ref="A137:E137"/>
+    <mergeCell ref="A146:E146"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>